<commit_message>
update ID0001 + logo.obj
</commit_message>
<xml_diff>
--- a/PlantillaExcelGestion.xlsx
+++ b/PlantillaExcelGestion.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7968F4-3A6D-414D-9860-519740531CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60B4BEE-42A6-4D54-AA16-31D35DC752AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="810" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="12" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Como Usuario quiero que modelos 3D se carguen desde BBDD para tener una experiencia fluida</t>
-  </si>
-  <si>
     <t>Como Usuario quiero visualizar estatuas de pokémons y cartas para reconocer emblemas de la saga</t>
   </si>
   <si>
@@ -280,18 +277,9 @@
     <t>ID0001_T4</t>
   </si>
   <si>
-    <t>Los modelos 3D se cargan dinámicamente desde la BBDD sin bloquear la interfaz</t>
-  </si>
-  <si>
     <t>Tiempo de carga &lt; 3 segundos en conexiones estándar</t>
   </si>
   <si>
-    <t>Soporte para formatos .fbx, .obj y texturas asociadas</t>
-  </si>
-  <si>
-    <t>Gestión de errores si un modelo no está disponible</t>
-  </si>
-  <si>
     <t>Texturas en alta resolución</t>
   </si>
   <si>
@@ -368,6 +356,18 @@
   </si>
   <si>
     <t>Un museo que invita a futuros empleados a descubrir la historia, innovación y valores de The Pokémon Company, conectándolos con la esencia y legado de esta icónica franquicia</t>
+  </si>
+  <si>
+    <t>Como Usuario quiero que modelos 3D se carguen desde repositorio público de GitHub</t>
+  </si>
+  <si>
+    <t>Integración en Unity</t>
+  </si>
+  <si>
+    <t>Configurar la carga de modelos desde GitHub</t>
+  </si>
+  <si>
+    <t>Gestión de errores y pruebas</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,13 +481,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -563,7 +556,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -948,13 +941,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1151,9 +1224,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1169,6 +1239,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1211,13 +1329,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1357,31 +1475,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.8</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.7</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.6</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.4</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.299999999999997</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.199999999999996</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0999999999999943</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1412,7 +1530,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2113,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2126,7 +2244,7 @@
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="58" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
@@ -2138,10 +2256,10 @@
     </row>
     <row r="4" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14"/>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="97"/>
+      <c r="C4" s="112"/>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
@@ -2252,10 +2370,10 @@
     </row>
     <row r="12" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="97"/>
+      <c r="C12" s="112"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
@@ -2296,13 +2414,13 @@
       <c r="E14" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="103"/>
+      <c r="F14" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="117"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="118"/>
       <c r="K14" s="83"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2319,13 +2437,13 @@
       <c r="E15" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="106"/>
+      <c r="F15" s="119" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="121"/>
       <c r="K15" s="87"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2345,25 +2463,25 @@
       <c r="A17" s="14"/>
     </row>
     <row r="18" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="100"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="93" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="95"/>
+      <c r="B19" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2437,7 +2555,7 @@
       </c>
       <c r="E2" s="21">
         <f>SUM(E3:E6)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -2448,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C3" s="8">
         <v>100</v>
@@ -2457,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="8"/>
       <c r="H3" s="3"/>
@@ -2467,7 +2585,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="8">
         <v>90</v>
@@ -2487,7 +2605,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="8">
         <v>80</v>
@@ -2507,7 +2625,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="8">
         <v>70</v>
@@ -2523,29 +2641,29 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="89"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="92">
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="91">
         <f>AVERAGE(C8:C12)</f>
         <v>46</v>
       </c>
-      <c r="D7" s="92">
+      <c r="D7" s="91">
         <v>2</v>
       </c>
-      <c r="E7" s="92">
+      <c r="E7" s="91">
         <f>SUM(E8:E12)</f>
         <v>33</v>
       </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="88"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="8">
         <v>80</v>
@@ -2565,7 +2683,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="8">
         <v>60</v>
@@ -2585,7 +2703,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="8">
         <v>40</v>
@@ -2605,7 +2723,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="8">
         <v>30</v>
@@ -2625,7 +2743,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="76">
         <v>20</v>
@@ -2684,7 +2802,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2716,7 +2834,7 @@
       <c r="B2" s="27"/>
       <c r="C2" s="27">
         <f>SUM(C3,C8,C12,C16,C19,C22,C25,C28,C33)</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="40"/>
@@ -2726,11 +2844,11 @@
         <v>4</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C3" s="13">
         <f>SUM(C4:C7)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="12"/>
     </row>
@@ -2739,10 +2857,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2750,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
@@ -2761,7 +2879,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
@@ -2769,10 +2887,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
@@ -2783,7 +2901,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="13">
         <f>SUM(C9:C11)</f>
@@ -2796,7 +2914,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -2807,7 +2925,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -2818,7 +2936,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -2829,7 +2947,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="13">
         <f>SUM(C13:C15)</f>
@@ -2842,7 +2960,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2853,7 +2971,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -2861,10 +2979,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -2875,7 +2993,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="13">
         <f>SUM(C17:C18)</f>
@@ -2888,7 +3006,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -2899,7 +3017,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -2910,7 +3028,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="13">
         <f>SUM(C20:C21)</f>
@@ -2923,7 +3041,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2">
         <v>6</v>
@@ -2934,7 +3052,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2">
         <v>2</v>
@@ -2945,7 +3063,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="13">
         <f>SUM(C23:C24)</f>
@@ -2958,7 +3076,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2">
         <v>3</v>
@@ -2969,7 +3087,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
@@ -2980,7 +3098,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="13">
         <f>SUM(C26:C27)</f>
@@ -2993,7 +3111,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2">
         <v>3</v>
@@ -3004,7 +3122,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2">
         <v>2</v>
@@ -3015,7 +3133,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="13">
         <f>SUM(C29:C32)</f>
@@ -3028,7 +3146,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2">
         <v>4</v>
@@ -3039,7 +3157,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2">
         <v>3</v>
@@ -3050,7 +3168,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2">
         <v>3</v>
@@ -3061,7 +3179,7 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2">
         <v>3</v>
@@ -3072,7 +3190,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="13">
         <f>SUM(C34:C36)</f>
@@ -3085,7 +3203,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -3096,7 +3214,7 @@
         <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C35" s="2">
         <v>0.5</v>
@@ -3107,7 +3225,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C36" s="2">
         <v>0.5</v>
@@ -3277,18 +3395,18 @@
       <c r="N5" s="43"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="109"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="124"/>
       <c r="D6" s="36">
         <f>COUNTIF(D10:D899,"&gt;0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="44">
         <f t="shared" ref="E6:N6" si="2">COUNTIF(E10:E932,"&gt;0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="44">
         <f t="shared" si="2"/>
@@ -3328,18 +3446,18 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="122" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="124"/>
       <c r="D7" s="38">
         <f>SUM(D9:D932)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="45">
         <f>IF(SUM(E10:E42)&gt;=0,SUM(E10:E42),#N/A)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="45">
         <f t="shared" ref="F7:N7" si="3">IF(SUM(F10:F42)&gt;=0,SUM(F10:F42),#N/A)</f>
@@ -3379,301 +3497,305 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="110" t="s">
+      <c r="E9" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="112"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="127"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="106">
+        <v>3</v>
+      </c>
+      <c r="E10" s="106">
+        <v>2</v>
+      </c>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="106"/>
+      <c r="N10" s="107"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="108"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="108"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="108"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="108"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="108"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="108"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="108"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="108"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="108"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="108"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="C21" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="109"/>
+      <c r="N21" s="110"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>66</v>
@@ -3695,7 +3817,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>66</v>
@@ -3717,7 +3839,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>66</v>
@@ -3739,7 +3861,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>66</v>
@@ -3761,7 +3883,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>66</v>
@@ -3783,7 +3905,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>66</v>
@@ -3805,7 +3927,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>66</v>
@@ -3827,7 +3949,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>66</v>
@@ -3849,7 +3971,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>66</v>
@@ -3871,7 +3993,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>66</v>
@@ -3893,7 +4015,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>66</v>
@@ -3915,7 +4037,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>66</v>
@@ -3937,7 +4059,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>66</v>
@@ -4253,11 +4375,11 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="109"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="124"/>
       <c r="D6" s="36"/>
       <c r="E6" s="37">
         <f>SUM($E$10:E42)</f>
@@ -4301,11 +4423,11 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="109"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="124"/>
       <c r="D7" s="38">
         <f>SUM(E7:N7)</f>
         <v>0</v>
@@ -4364,289 +4486,319 @@
       <c r="D9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="115"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="129"/>
+      <c r="L9" s="129"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="130"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="100"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="101"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="98" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="N11" s="102"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="N12" s="102"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="N13" s="102"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="N14" s="102"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="N15" s="102"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="N16" s="102"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="N17" s="102"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="N18" s="102"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="N19" s="102"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="N20" s="102"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="103"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="104"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>66</v>
@@ -4658,7 +4810,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>66</v>
@@ -4670,7 +4822,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>66</v>
@@ -4774,7 +4926,7 @@
       </c>
       <c r="B27" s="48">
         <f>'Pila-Sprint1'!C2</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="33">
         <v>42278</v>
@@ -4814,43 +4966,43 @@
       <c r="B28" s="35"/>
       <c r="C28" s="35">
         <f>$B$27/10</f>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="D28" s="35">
         <f t="shared" ref="D28:L28" si="0">$B$27/10</f>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="E28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="F28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="G28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="H28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="J28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="K28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="L28" s="35">
         <f t="shared" si="0"/>
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="M28" s="35"/>
       <c r="N28" s="35"/>
@@ -4865,39 +5017,39 @@
       <c r="B29" s="35"/>
       <c r="C29" s="35">
         <f>B27</f>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="35">
         <f>$B$27-SUM($C$28:D28)</f>
-        <v>48.8</v>
+        <v>48</v>
       </c>
       <c r="E29" s="35">
         <f>$B$27-SUM($C$28:E28)</f>
-        <v>42.7</v>
+        <v>42</v>
       </c>
       <c r="F29" s="35">
         <f>$B$27-SUM($C$28:F28)</f>
-        <v>36.6</v>
+        <v>36</v>
       </c>
       <c r="G29" s="35">
         <f>$B$27-SUM($C$28:G28)</f>
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="H29" s="35">
         <f>$B$27-SUM($C$28:H28)</f>
-        <v>24.4</v>
+        <v>24</v>
       </c>
       <c r="I29" s="35">
         <f>$B$27-SUM($C$28:I28)</f>
-        <v>18.299999999999997</v>
+        <v>18</v>
       </c>
       <c r="J29" s="35">
         <f>$B$27-SUM($C$28:J28)</f>
-        <v>12.199999999999996</v>
+        <v>12</v>
       </c>
       <c r="K29" s="35">
         <f>$B$27-SUM($C$28:K28)</f>
-        <v>6.0999999999999943</v>
+        <v>6</v>
       </c>
       <c r="L29" s="35">
         <f>$B$27-SUM($C$28:L28)</f>
@@ -4919,7 +5071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
update 20/10/2025 (clean models)
</commit_message>
<xml_diff>
--- a/PlantillaExcelGestion.xlsx
+++ b/PlantillaExcelGestion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60B4BEE-42A6-4D54-AA16-31D35DC752AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3038F3B8-D6B5-494A-ADDD-715AA3DED6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1530,10 +1530,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1709,34 +1709,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2239,7 +2239,7 @@
     <col min="4" max="4" width="17.109375" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="50.77734375" customWidth="1"/>
+    <col min="11" max="11" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
@@ -3402,15 +3402,15 @@
       <c r="C6" s="124"/>
       <c r="D6" s="36">
         <f>COUNTIF(D10:D899,"&gt;0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="44">
         <f t="shared" ref="E6:N6" si="2">COUNTIF(E10:E932,"&gt;0")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="44">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="44">
         <f t="shared" si="2"/>
@@ -3453,15 +3453,15 @@
       <c r="C7" s="124"/>
       <c r="D7" s="38">
         <f>SUM(D9:D932)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7" s="45">
         <f>IF(SUM(E10:E42)&gt;=0,SUM(E10:E42),#N/A)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F7" s="45">
         <f t="shared" ref="F7:N7" si="3">IF(SUM(F10:F42)&gt;=0,SUM(F10:F42),#N/A)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="45">
         <f t="shared" si="3"/>
@@ -3538,7 +3538,9 @@
       <c r="E10" s="106">
         <v>2</v>
       </c>
-      <c r="F10" s="106"/>
+      <c r="F10" s="106">
+        <v>1</v>
+      </c>
       <c r="G10" s="106"/>
       <c r="H10" s="106"/>
       <c r="I10" s="106"/>
@@ -3556,10 +3558,14 @@
         <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+        <v>57</v>
+      </c>
+      <c r="D11" s="20">
+        <v>3</v>
+      </c>
+      <c r="E11" s="20">
+        <v>2</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -4383,43 +4389,43 @@
       <c r="D6" s="36"/>
       <c r="E6" s="37">
         <f>SUM($E$10:E42)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="37">
         <f>SUM($E$7:F7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="37">
         <f>SUM($E$7:G7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="37">
         <f>SUM($E$7:H7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6" s="37">
         <f>SUM($E$7:I7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J6" s="37">
         <f>SUM($E$7:J7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K6" s="37">
         <f>SUM($E$7:K7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" s="37">
         <f>SUM($E$7:L7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6" s="37">
         <f>SUM($E$7:M7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N6" s="37">
         <f>SUM($E$7:N7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4430,15 +4436,15 @@
       <c r="C7" s="124"/>
       <c r="D7" s="38">
         <f>SUM(E7:N7)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="39">
         <f>SUM(E10:E42)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="39">
         <f t="shared" ref="F7:N7" si="2">SUM(F10:F42)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="39">
         <f t="shared" si="2"/>
@@ -4507,11 +4513,17 @@
         <v>109</v>
       </c>
       <c r="C10" s="97" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
+        <v>57</v>
+      </c>
+      <c r="D10" s="100">
+        <v>3</v>
+      </c>
+      <c r="E10" s="97">
+        <v>2</v>
+      </c>
+      <c r="F10" s="97">
+        <v>1</v>
+      </c>
       <c r="G10" s="97"/>
       <c r="H10" s="97"/>
       <c r="I10" s="97"/>

</xml_diff>

<commit_message>
pictures + new models - update 09/11/2025
</commit_message>
<xml_diff>
--- a/PlantillaExcelGestion.xlsx
+++ b/PlantillaExcelGestion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CC8561-E0C3-4B3A-8F0E-0AAC17D4873F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B7CD8C-C0B2-4059-85D9-7D6C3C54719E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1128" yWindow="2196" windowWidth="21912" windowHeight="8964" tabRatio="810" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="12" r:id="rId1"/>
@@ -1031,7 +1031,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1233,9 +1233,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1317,13 +1314,13 @@
     <xf numFmtId="166" fontId="3" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3060,9 +3057,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3100,9 +3097,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3135,26 +3132,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3187,26 +3167,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3384,16 +3347,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="57" t="s">
         <v>97</v>
       </c>
@@ -3401,18 +3364,18 @@
       <c r="D2" s="58"/>
       <c r="E2" s="59"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="105"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="104"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="53" t="s">
         <v>1</v>
@@ -3431,7 +3394,7 @@
       <c r="J5" s="55"/>
       <c r="K5" s="54"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="62" t="s">
         <v>66</v>
@@ -3448,7 +3411,7 @@
       <c r="J6" s="61"/>
       <c r="K6" s="63"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="64" t="s">
         <v>65</v>
@@ -3465,7 +3428,7 @@
       <c r="J7" s="60"/>
       <c r="K7" s="65"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="69" t="s">
         <v>66</v>
@@ -3482,7 +3445,7 @@
       <c r="J8" s="70"/>
       <c r="K8" s="71"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="69" t="s">
         <v>67</v>
@@ -3499,7 +3462,7 @@
       <c r="J9" s="70"/>
       <c r="K9" s="71"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="66" t="s">
         <v>65</v>
@@ -3516,17 +3479,17 @@
       <c r="J10" s="67"/>
       <c r="K10" s="68"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="105"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="104"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="52" t="s">
         <v>8</v>
@@ -3551,7 +3514,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="79" t="s">
         <v>40</v>
@@ -3562,22 +3525,22 @@
       <c r="D14" s="78">
         <v>45964</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="91">
         <f>21/28</f>
         <v>0.75</v>
       </c>
-      <c r="F14" s="109" t="s">
+      <c r="F14" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="93" t="s">
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="92" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="80" t="s">
         <v>68</v>
@@ -3591,16 +3554,16 @@
       <c r="E15" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="112" t="s">
+      <c r="F15" s="111" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="114"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="113"/>
       <c r="K15" s="83"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="75"/>
       <c r="C16" s="75"/>
@@ -3613,17 +3576,17 @@
       <c r="J16" s="75"/>
       <c r="K16" s="75"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
     </row>
-    <row r="18" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="106" t="s">
+    <row r="18" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="107"/>
-      <c r="D18" s="108"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="106"/>
+      <c r="D18" s="107"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="86" t="s">
         <v>100</v>
       </c>
@@ -3660,19 +3623,19 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="164" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3698,7 +3661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20">
@@ -3717,14 +3680,14 @@
         <f>SUM(F3:F6)</f>
         <v>32</v>
       </c>
-      <c r="G2" s="100">
+      <c r="G2" s="99">
         <f>COUNTIF(G3:G6,"finished")/COUNTIF(G3:G6,"&lt;&gt;"&amp;"")</f>
         <v>0.5</v>
       </c>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="93" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -3750,8 +3713,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="94" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -3770,15 +3733,15 @@
         <f>SUM('Diario-Realizado'!D13:D14)</f>
         <v>10</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="97" t="s">
         <v>108</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="94" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -3797,15 +3760,15 @@
         <f>SUM('Diario-Realizado'!D15:D17)</f>
         <v>8</v>
       </c>
-      <c r="G5" s="99" t="s">
+      <c r="G5" s="98" t="s">
         <v>108</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="93" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -3824,12 +3787,12 @@
         <f>SUM('Diario-Realizado'!D18)</f>
         <v>2</v>
       </c>
-      <c r="G6" s="99" t="s">
+      <c r="G6" s="98" t="s">
         <v>107</v>
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="85">
@@ -3847,14 +3810,14 @@
         <f>SUM(F8:F12)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="100">
         <f>COUNTIF(G8:G12,"finished")/COUNTIF(G8:G12,"&lt;&gt;"&amp;"")</f>
         <v>0</v>
       </c>
       <c r="H7" s="84"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="96" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="95" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -3870,13 +3833,13 @@
         <v>6</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="99" t="s">
+      <c r="G8" s="98" t="s">
         <v>108</v>
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="96" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="95" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -3892,13 +3855,13 @@
         <v>4</v>
       </c>
       <c r="F9" s="74"/>
-      <c r="G9" s="99" t="s">
+      <c r="G9" s="98" t="s">
         <v>108</v>
       </c>
       <c r="H9" s="73"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="96" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="95" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3914,13 +3877,13 @@
         <v>4</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="99" t="s">
+      <c r="G10" s="98" t="s">
         <v>108</v>
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="95" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -3936,13 +3899,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="99" t="s">
+      <c r="G11" s="98" t="s">
         <v>108</v>
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="97" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="96" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="73" t="s">
@@ -3963,29 +3926,29 @@
       </c>
       <c r="H12" s="73"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="19"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" s="19"/>
     </row>
   </sheetData>
@@ -4011,17 +3974,17 @@
       <selection activeCell="A16" sqref="A16:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="131.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="131.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -4036,7 +3999,7 @@
       </c>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" s="23" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26">
@@ -4046,7 +4009,7 @@
       <c r="D2" s="27"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -4059,7 +4022,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -4070,7 +4033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -4084,7 +4047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4098,7 +4061,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -4111,7 +4074,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -4122,7 +4085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -4133,7 +4096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -4146,7 +4109,7 @@
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -4157,7 +4120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -4168,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -4179,7 +4142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
@@ -4192,7 +4155,7 @@
       </c>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -4203,7 +4166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>10</v>
       </c>
@@ -4215,7 +4178,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -4223,7 +4186,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -4231,7 +4194,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -4243,7 +4206,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4251,7 +4214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -4259,7 +4222,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
@@ -4271,7 +4234,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -4279,7 +4242,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -4287,7 +4250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>28</v>
       </c>
@@ -4299,7 +4262,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -4307,7 +4270,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -4315,7 +4278,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -4323,7 +4286,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -4331,7 +4294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
@@ -4343,7 +4306,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -4351,7 +4314,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -4359,7 +4322,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -4382,17 +4345,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="131.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="131.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="23" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -4407,7 +4370,7 @@
       </c>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" s="23" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26">
@@ -4417,7 +4380,7 @@
       <c r="D2" s="27"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -4430,7 +4393,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -4441,7 +4404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -4455,7 +4418,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4469,7 +4432,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -4482,7 +4445,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -4493,7 +4456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -4504,7 +4467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -4517,7 +4480,7 @@
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -4528,7 +4491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -4539,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -4550,7 +4513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>7</v>
       </c>
@@ -4563,7 +4526,7 @@
       </c>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -4574,7 +4537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>10</v>
       </c>
@@ -4587,7 +4550,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -4598,7 +4561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -4609,7 +4572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -4622,7 +4585,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -4633,7 +4596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -4644,7 +4607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>11</v>
       </c>
@@ -4657,7 +4620,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -4668,7 +4631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -4679,7 +4642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>28</v>
       </c>
@@ -4692,7 +4655,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -4703,7 +4666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -4714,7 +4677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -4725,7 +4688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -4736,7 +4699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
@@ -4749,7 +4712,7 @@
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -4760,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -4771,7 +4734,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -4797,18 +4760,18 @@
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="14" width="5.7109375" style="45" customWidth="1"/>
-    <col min="15" max="55" width="5.7109375" style="1" customWidth="1"/>
-    <col min="56" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="14" width="5.6640625" style="45" customWidth="1"/>
+    <col min="15" max="55" width="5.6640625" style="1" customWidth="1"/>
+    <col min="56" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" s="49"/>
       <c r="B2" s="49"/>
       <c r="C2" s="28"/>
@@ -4824,7 +4787,7 @@
       <c r="M2" s="40"/>
       <c r="N2" s="40"/>
     </row>
-    <row r="3" spans="1:55" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50"/>
       <c r="B3" s="51"/>
       <c r="C3" s="28"/>
@@ -5034,7 +4997,7 @@
         <v>M</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -5193,7 +5156,7 @@
         <v>42332</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -5274,12 +5237,12 @@
       <c r="BB5" s="42"/>
       <c r="BC5" s="42"/>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
+    <row r="6" spans="1:55" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="116"/>
-      <c r="C6" s="117"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="116"/>
       <c r="D6" s="35">
         <f>COUNTIF(D10:D896,"&gt;0")</f>
         <v>9</v>
@@ -5489,12 +5452,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
+    <row r="7" spans="1:55" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="117"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="37">
         <f>SUM(D9:D929)</f>
         <v>23</v>
@@ -5704,7 +5667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="89" t="s">
         <v>0</v>
       </c>
@@ -5717,61 +5680,61 @@
       <c r="D9" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="118" t="s">
+      <c r="E9" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119"/>
-      <c r="T9" s="119"/>
-      <c r="U9" s="119"/>
-      <c r="V9" s="119"/>
-      <c r="W9" s="119"/>
-      <c r="X9" s="119"/>
-      <c r="Y9" s="119"/>
-      <c r="Z9" s="119"/>
-      <c r="AA9" s="119"/>
-      <c r="AB9" s="119"/>
-      <c r="AC9" s="119"/>
-      <c r="AD9" s="119"/>
-      <c r="AE9" s="119"/>
-      <c r="AF9" s="119"/>
-      <c r="AG9" s="119"/>
-      <c r="AH9" s="119"/>
-      <c r="AI9" s="119"/>
-      <c r="AJ9" s="119"/>
-      <c r="AK9" s="119"/>
-      <c r="AL9" s="119"/>
-      <c r="AM9" s="119"/>
-      <c r="AN9" s="119"/>
-      <c r="AO9" s="119"/>
-      <c r="AP9" s="119"/>
-      <c r="AQ9" s="119"/>
-      <c r="AR9" s="119"/>
-      <c r="AS9" s="119"/>
-      <c r="AT9" s="119"/>
-      <c r="AU9" s="119"/>
-      <c r="AV9" s="119"/>
-      <c r="AW9" s="119"/>
-      <c r="AX9" s="119"/>
-      <c r="AY9" s="119"/>
-      <c r="AZ9" s="119"/>
-      <c r="BA9" s="119"/>
-      <c r="BB9" s="119"/>
-      <c r="BC9" s="119"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
+      <c r="Q9" s="118"/>
+      <c r="R9" s="118"/>
+      <c r="S9" s="118"/>
+      <c r="T9" s="118"/>
+      <c r="U9" s="118"/>
+      <c r="V9" s="118"/>
+      <c r="W9" s="118"/>
+      <c r="X9" s="118"/>
+      <c r="Y9" s="118"/>
+      <c r="Z9" s="118"/>
+      <c r="AA9" s="118"/>
+      <c r="AB9" s="118"/>
+      <c r="AC9" s="118"/>
+      <c r="AD9" s="118"/>
+      <c r="AE9" s="118"/>
+      <c r="AF9" s="118"/>
+      <c r="AG9" s="118"/>
+      <c r="AH9" s="118"/>
+      <c r="AI9" s="118"/>
+      <c r="AJ9" s="118"/>
+      <c r="AK9" s="118"/>
+      <c r="AL9" s="118"/>
+      <c r="AM9" s="118"/>
+      <c r="AN9" s="118"/>
+      <c r="AO9" s="118"/>
+      <c r="AP9" s="118"/>
+      <c r="AQ9" s="118"/>
+      <c r="AR9" s="118"/>
+      <c r="AS9" s="118"/>
+      <c r="AT9" s="118"/>
+      <c r="AU9" s="118"/>
+      <c r="AV9" s="118"/>
+      <c r="AW9" s="118"/>
+      <c r="AX9" s="118"/>
+      <c r="AY9" s="118"/>
+      <c r="AZ9" s="118"/>
+      <c r="BA9" s="118"/>
+      <c r="BB9" s="118"/>
+      <c r="BC9" s="118"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" s="90" t="s">
         <v>113</v>
       </c>
@@ -5781,7 +5744,7 @@
       <c r="C10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="102">
+      <c r="D10" s="101">
         <f>'Pila-Sprint1'!C4</f>
         <v>4</v>
       </c>
@@ -5939,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" s="90" t="s">
         <v>115</v>
       </c>
@@ -6107,7 +6070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
         <v>114</v>
       </c>
@@ -6275,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
         <v>15</v>
       </c>
@@ -6443,7 +6406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
         <v>16</v>
       </c>
@@ -6611,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" s="90" t="s">
         <v>17</v>
       </c>
@@ -6779,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" s="90" t="s">
         <v>18</v>
       </c>
@@ -6947,7 +6910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -7115,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A18" s="90" t="s">
         <v>19</v>
       </c>
@@ -7283,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A19" s="90" t="s">
         <v>20</v>
       </c>
@@ -7451,7 +7414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A20" s="90" t="s">
         <v>21</v>
       </c>
@@ -7619,7 +7582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A21" s="90" t="s">
         <v>22</v>
       </c>
@@ -7787,7 +7750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A22" s="90" t="s">
         <v>23</v>
       </c>
@@ -7955,7 +7918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A23" s="90" t="s">
         <v>24</v>
       </c>
@@ -8123,7 +8086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A24" s="90" t="s">
         <v>25</v>
       </c>
@@ -8291,7 +8254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A25" s="90" t="s">
         <v>116</v>
       </c>
@@ -8459,7 +8422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A26" s="90" t="s">
         <v>117</v>
       </c>
@@ -8627,7 +8590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A27" s="90" t="s">
         <v>118</v>
       </c>
@@ -8795,7 +8758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A28" s="90" t="s">
         <v>119</v>
       </c>
@@ -8963,7 +8926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A29" s="90" t="s">
         <v>120</v>
       </c>
@@ -9131,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A30" s="90" t="s">
         <v>121</v>
       </c>
@@ -9299,7 +9262,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A31" s="90" t="s">
         <v>122</v>
       </c>
@@ -9467,7 +9430,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -9480,7 +9443,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -9493,7 +9456,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -9506,7 +9469,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -9519,7 +9482,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -9532,7 +9495,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -9545,7 +9508,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -9558,7 +9521,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -9571,7 +9534,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -9610,19 +9573,19 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="55" width="5.7109375" style="1" customWidth="1"/>
-    <col min="56" max="57" width="11.42578125" style="1"/>
-    <col min="58" max="58" width="5.7109375" style="1" customWidth="1"/>
-    <col min="59" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="55" width="5.6640625" style="1" customWidth="1"/>
+    <col min="56" max="57" width="11.44140625" style="1"/>
+    <col min="58" max="58" width="5.6640625" style="1" customWidth="1"/>
+    <col min="59" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" s="49"/>
       <c r="B2" s="49"/>
       <c r="C2" s="28"/>
@@ -9638,7 +9601,7 @@
       <c r="M2" s="28"/>
       <c r="N2" s="28"/>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" s="50"/>
       <c r="B3" s="51"/>
       <c r="C3" s="28"/>
@@ -9848,7 +9811,7 @@
         <v>M</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="37.799999999999997" x14ac:dyDescent="0.3">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -10007,7 +9970,7 @@
         <v>42332</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -10214,12 +10177,12 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="115" t="s">
+    <row r="6" spans="1:55" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="116"/>
-      <c r="C6" s="117"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="116"/>
       <c r="D6" s="35"/>
       <c r="E6" s="36">
         <f>SUM($E$10:E16)</f>
@@ -10426,12 +10389,12 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="115" t="s">
+    <row r="7" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="117"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="37">
         <f>SUM(E7:N7)</f>
         <v>2</v>
@@ -10641,7 +10604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:55" s="23" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>0</v>
       </c>
@@ -10654,61 +10617,61 @@
       <c r="D9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="120" t="s">
+      <c r="E9" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="121"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="121"/>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="121"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="121"/>
-      <c r="T9" s="121"/>
-      <c r="U9" s="121"/>
-      <c r="V9" s="121"/>
-      <c r="W9" s="121"/>
-      <c r="X9" s="121"/>
-      <c r="Y9" s="121"/>
-      <c r="Z9" s="121"/>
-      <c r="AA9" s="121"/>
-      <c r="AB9" s="121"/>
-      <c r="AC9" s="121"/>
-      <c r="AD9" s="121"/>
-      <c r="AE9" s="121"/>
-      <c r="AF9" s="121"/>
-      <c r="AG9" s="121"/>
-      <c r="AH9" s="121"/>
-      <c r="AI9" s="121"/>
-      <c r="AJ9" s="121"/>
-      <c r="AK9" s="121"/>
-      <c r="AL9" s="121"/>
-      <c r="AM9" s="121"/>
-      <c r="AN9" s="121"/>
-      <c r="AO9" s="121"/>
-      <c r="AP9" s="121"/>
-      <c r="AQ9" s="121"/>
-      <c r="AR9" s="121"/>
-      <c r="AS9" s="121"/>
-      <c r="AT9" s="121"/>
-      <c r="AU9" s="121"/>
-      <c r="AV9" s="121"/>
-      <c r="AW9" s="121"/>
-      <c r="AX9" s="121"/>
-      <c r="AY9" s="121"/>
-      <c r="AZ9" s="121"/>
-      <c r="BA9" s="121"/>
-      <c r="BB9" s="121"/>
-      <c r="BC9" s="121"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="120"/>
+      <c r="Q9" s="120"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="120"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="120"/>
+      <c r="V9" s="120"/>
+      <c r="W9" s="120"/>
+      <c r="X9" s="120"/>
+      <c r="Y9" s="120"/>
+      <c r="Z9" s="120"/>
+      <c r="AA9" s="120"/>
+      <c r="AB9" s="120"/>
+      <c r="AC9" s="120"/>
+      <c r="AD9" s="120"/>
+      <c r="AE9" s="120"/>
+      <c r="AF9" s="120"/>
+      <c r="AG9" s="120"/>
+      <c r="AH9" s="120"/>
+      <c r="AI9" s="120"/>
+      <c r="AJ9" s="120"/>
+      <c r="AK9" s="120"/>
+      <c r="AL9" s="120"/>
+      <c r="AM9" s="120"/>
+      <c r="AN9" s="120"/>
+      <c r="AO9" s="120"/>
+      <c r="AP9" s="120"/>
+      <c r="AQ9" s="120"/>
+      <c r="AR9" s="120"/>
+      <c r="AS9" s="120"/>
+      <c r="AT9" s="120"/>
+      <c r="AU9" s="120"/>
+      <c r="AV9" s="120"/>
+      <c r="AW9" s="120"/>
+      <c r="AX9" s="120"/>
+      <c r="AY9" s="120"/>
+      <c r="AZ9" s="120"/>
+      <c r="BA9" s="120"/>
+      <c r="BB9" s="120"/>
+      <c r="BC9" s="120"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10" s="90" t="s">
         <v>113</v>
       </c>
@@ -10778,7 +10741,7 @@
       <c r="BB10" s="19"/>
       <c r="BC10" s="19"/>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11" s="90" t="s">
         <v>115</v>
       </c>
@@ -10848,7 +10811,7 @@
       <c r="BB11" s="19"/>
       <c r="BC11" s="19"/>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
         <v>114</v>
       </c>
@@ -10916,7 +10879,7 @@
       <c r="BB12" s="19"/>
       <c r="BC12" s="19"/>
     </row>
-    <row r="13" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="90" t="s">
         <v>15</v>
       </c>
@@ -10984,7 +10947,7 @@
       <c r="BB13" s="19"/>
       <c r="BC13" s="19"/>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
         <v>16</v>
       </c>
@@ -11058,7 +11021,7 @@
       <c r="BB14" s="19"/>
       <c r="BC14" s="19"/>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A15" s="90" t="s">
         <v>17</v>
       </c>
@@ -11128,7 +11091,7 @@
       <c r="BB15" s="19"/>
       <c r="BC15" s="19"/>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A16" s="90" t="s">
         <v>18</v>
       </c>
@@ -11196,7 +11159,7 @@
       <c r="BB16" s="19"/>
       <c r="BC16" s="19"/>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -11264,7 +11227,7 @@
       <c r="BB17" s="19"/>
       <c r="BC17" s="19"/>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A18" s="90" t="s">
         <v>19</v>
       </c>
@@ -11332,7 +11295,7 @@
       <c r="BB18" s="19"/>
       <c r="BC18" s="19"/>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A19" s="90" t="s">
         <v>20</v>
       </c>
@@ -11398,7 +11361,7 @@
       <c r="BB19" s="19"/>
       <c r="BC19" s="19"/>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A20" s="90" t="s">
         <v>21</v>
       </c>
@@ -11464,7 +11427,7 @@
       <c r="BB20" s="19"/>
       <c r="BC20" s="19"/>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A21" s="90" t="s">
         <v>22</v>
       </c>
@@ -11530,7 +11493,7 @@
       <c r="BB21" s="19"/>
       <c r="BC21" s="19"/>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A22" s="90" t="s">
         <v>23</v>
       </c>
@@ -11596,7 +11559,7 @@
       <c r="BB22" s="19"/>
       <c r="BC22" s="19"/>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A23" s="90" t="s">
         <v>24</v>
       </c>
@@ -11662,7 +11625,7 @@
       <c r="BB23" s="19"/>
       <c r="BC23" s="19"/>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A24" s="90" t="s">
         <v>25</v>
       </c>
@@ -11728,7 +11691,7 @@
       <c r="BB24" s="19"/>
       <c r="BC24" s="19"/>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A25" s="90" t="s">
         <v>116</v>
       </c>
@@ -11794,7 +11757,7 @@
       <c r="BB25" s="19"/>
       <c r="BC25" s="19"/>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A26" s="90" t="s">
         <v>117</v>
       </c>
@@ -11860,7 +11823,7 @@
       <c r="BB26" s="19"/>
       <c r="BC26" s="19"/>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A27" s="90" t="s">
         <v>118</v>
       </c>
@@ -11926,7 +11889,7 @@
       <c r="BB27" s="19"/>
       <c r="BC27" s="19"/>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A28" s="90" t="s">
         <v>119</v>
       </c>
@@ -11992,7 +11955,7 @@
       <c r="BB28" s="19"/>
       <c r="BC28" s="19"/>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A29" s="90" t="s">
         <v>120</v>
       </c>
@@ -12058,7 +12021,7 @@
       <c r="BB29" s="19"/>
       <c r="BC29" s="19"/>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A30" s="90" t="s">
         <v>121</v>
       </c>
@@ -12124,7 +12087,7 @@
       <c r="BB30" s="19"/>
       <c r="BC30" s="19"/>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A31" s="90" t="s">
         <v>122</v>
       </c>
@@ -12190,7 +12153,7 @@
       <c r="BB31" s="19"/>
       <c r="BC31" s="19"/>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -12243,7 +12206,7 @@
       <c r="BB32" s="19"/>
       <c r="BC32" s="19"/>
     </row>
-    <row r="33" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
@@ -12296,7 +12259,7 @@
       <c r="BB33" s="19"/>
       <c r="BC33" s="19"/>
     </row>
-    <row r="34" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -12349,7 +12312,7 @@
       <c r="BB34" s="19"/>
       <c r="BC34" s="19"/>
     </row>
-    <row r="35" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
@@ -12402,7 +12365,7 @@
       <c r="BB35" s="19"/>
       <c r="BC35" s="19"/>
     </row>
-    <row r="36" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
@@ -12455,7 +12418,7 @@
       <c r="BB36" s="19"/>
       <c r="BC36" s="19"/>
     </row>
-    <row r="37" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
@@ -12508,7 +12471,7 @@
       <c r="BB37" s="19"/>
       <c r="BC37" s="19"/>
     </row>
-    <row r="38" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
@@ -12561,7 +12524,7 @@
       <c r="BB38" s="19"/>
       <c r="BC38" s="19"/>
     </row>
-    <row r="39" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
@@ -12614,7 +12577,7 @@
       <c r="BB39" s="19"/>
       <c r="BC39" s="19"/>
     </row>
-    <row r="40" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
@@ -12667,7 +12630,7 @@
       <c r="BB40" s="19"/>
       <c r="BC40" s="19"/>
     </row>
-    <row r="41" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -12720,7 +12683,7 @@
       <c r="BB41" s="19"/>
       <c r="BC41" s="19"/>
     </row>
-    <row r="42" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -12773,7 +12736,7 @@
       <c r="BB42" s="19"/>
       <c r="BC42" s="19"/>
     </row>
-    <row r="43" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -12826,7 +12789,7 @@
       <c r="BB43" s="19"/>
       <c r="BC43" s="19"/>
     </row>
-    <row r="44" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -12879,7 +12842,7 @@
       <c r="BB44" s="19"/>
       <c r="BC44" s="19"/>
     </row>
-    <row r="45" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -12932,7 +12895,7 @@
       <c r="BB45" s="19"/>
       <c r="BC45" s="19"/>
     </row>
-    <row r="46" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -12984,7 +12947,7 @@
       <c r="BA46" s="2"/>
       <c r="BB46" s="2"/>
     </row>
-    <row r="47" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -13036,7 +12999,7 @@
       <c r="BA47" s="2"/>
       <c r="BB47" s="2"/>
     </row>
-    <row r="48" spans="5:55" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:55" x14ac:dyDescent="0.3">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -13088,7 +13051,7 @@
       <c r="BA48" s="2"/>
       <c r="BB48" s="2"/>
     </row>
-    <row r="49" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -13140,7 +13103,7 @@
       <c r="BA49" s="2"/>
       <c r="BB49" s="2"/>
     </row>
-    <row r="50" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -13192,7 +13155,7 @@
       <c r="BA50" s="2"/>
       <c r="BB50" s="2"/>
     </row>
-    <row r="51" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -13244,7 +13207,7 @@
       <c r="BA51" s="2"/>
       <c r="BB51" s="2"/>
     </row>
-    <row r="52" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -13296,7 +13259,7 @@
       <c r="BA52" s="2"/>
       <c r="BB52" s="2"/>
     </row>
-    <row r="53" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -13348,7 +13311,7 @@
       <c r="BA53" s="2"/>
       <c r="BB53" s="2"/>
     </row>
-    <row r="54" spans="5:54" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:54" x14ac:dyDescent="0.3">
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -13426,34 +13389,34 @@
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="48" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="11" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="11" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E2"/>
     </row>
-    <row r="3" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E3"/>
     </row>
-    <row r="9" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E9"/>
     </row>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E12"/>
     </row>
-    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E14"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
         <v>47</v>
       </c>
@@ -13461,7 +13424,7 @@
       <c r="C26" s="46"/>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:32" ht="35.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" ht="36" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
         <v>48</v>
       </c>
@@ -13560,7 +13523,7 @@
         <v>42311</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="46" t="s">
         <v>49</v>
       </c>
@@ -13569,124 +13532,124 @@
         <f>$B$27/30</f>
         <v>0.76666666666666672</v>
       </c>
-      <c r="D28" s="91">
+      <c r="D28" s="34">
         <f t="shared" ref="D28:AF28" si="0">$B$27/30</f>
         <v>0.76666666666666672</v>
       </c>
-      <c r="E28" s="91">
+      <c r="E28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="F28" s="91">
+      <c r="F28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="G28" s="91">
+      <c r="G28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="H28" s="91">
+      <c r="H28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="I28" s="91">
+      <c r="I28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="J28" s="91">
+      <c r="J28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="K28" s="91">
+      <c r="K28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="L28" s="91">
+      <c r="L28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="M28" s="91">
+      <c r="M28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="N28" s="91">
+      <c r="N28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="O28" s="91">
+      <c r="O28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="P28" s="91">
+      <c r="P28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="Q28" s="91">
+      <c r="Q28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="R28" s="91">
+      <c r="R28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="S28" s="91">
+      <c r="S28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="T28" s="91">
+      <c r="T28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="U28" s="91">
+      <c r="U28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="V28" s="91">
+      <c r="V28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="W28" s="91">
+      <c r="W28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="X28" s="91">
+      <c r="X28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="Y28" s="91">
+      <c r="Y28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="Z28" s="91">
+      <c r="Z28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AA28" s="91">
+      <c r="AA28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AB28" s="91">
+      <c r="AB28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AC28" s="91">
+      <c r="AC28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AD28" s="91">
+      <c r="AD28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AE28" s="91">
+      <c r="AE28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="AF28" s="91">
+      <c r="AF28" s="34">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
     </row>
-    <row r="29" spans="1:32" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" ht="15" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
         <v>50</v>
       </c>
@@ -13703,111 +13666,111 @@
         <f>B27-SUM(C28:E28)</f>
         <v>20.7</v>
       </c>
-      <c r="F29" s="91">
+      <c r="F29" s="34">
         <f>B27-SUM(C28:F28)</f>
         <v>19.933333333333334</v>
       </c>
-      <c r="G29" s="91">
+      <c r="G29" s="34">
         <f>B27-SUM(C28:G28)</f>
         <v>19.166666666666668</v>
       </c>
-      <c r="H29" s="91">
+      <c r="H29" s="34">
         <f>B27-SUM(C28:H28)</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="I29" s="91">
+      <c r="I29" s="34">
         <f>B27-SUM(C28:I28)</f>
         <v>17.633333333333333</v>
       </c>
-      <c r="J29" s="91">
+      <c r="J29" s="34">
         <f>B27-SUM(C28:J28)</f>
         <v>16.866666666666667</v>
       </c>
-      <c r="K29" s="91">
+      <c r="K29" s="34">
         <f>B27-SUM(C28:K28)</f>
         <v>16.100000000000001</v>
       </c>
-      <c r="L29" s="91">
+      <c r="L29" s="34">
         <f>B27-SUM(C28:L28)</f>
         <v>15.333333333333332</v>
       </c>
-      <c r="M29" s="91">
+      <c r="M29" s="34">
         <f>B27-SUM(C28:M28)</f>
         <v>14.566666666666666</v>
       </c>
-      <c r="N29" s="91">
+      <c r="N29" s="34">
         <f>B27-SUM(C28:N28)</f>
         <v>13.799999999999999</v>
       </c>
-      <c r="O29" s="91">
+      <c r="O29" s="34">
         <f>B27-SUM(C28:O28)</f>
         <v>13.033333333333331</v>
       </c>
-      <c r="P29" s="91">
+      <c r="P29" s="34">
         <f>B27-SUM(C28:P28)</f>
         <v>12.266666666666664</v>
       </c>
-      <c r="Q29" s="91">
+      <c r="Q29" s="34">
         <f>B27-SUM(C28:Q28)</f>
         <v>11.499999999999996</v>
       </c>
-      <c r="R29" s="91">
+      <c r="R29" s="34">
         <f>B27-SUM(C28:R28)</f>
         <v>10.733333333333329</v>
       </c>
-      <c r="S29" s="91">
+      <c r="S29" s="34">
         <f>B27-SUM(C28:S28)</f>
         <v>9.9666666666666615</v>
       </c>
-      <c r="T29" s="91">
+      <c r="T29" s="34">
         <f>B27-SUM(C28:T28)</f>
         <v>9.199999999999994</v>
       </c>
-      <c r="U29" s="91">
+      <c r="U29" s="34">
         <f>B27-SUM(C28:U28)</f>
         <v>8.4333333333333265</v>
       </c>
-      <c r="V29" s="91">
+      <c r="V29" s="34">
         <f>B27-SUM(C28:V28)</f>
         <v>7.666666666666659</v>
       </c>
-      <c r="W29" s="91">
+      <c r="W29" s="34">
         <f>B27-SUM(C28:W28)</f>
         <v>6.8999999999999915</v>
       </c>
-      <c r="X29" s="91">
+      <c r="X29" s="34">
         <f>B27-SUM(C28:X28)</f>
         <v>6.1333333333333258</v>
       </c>
-      <c r="Y29" s="91">
+      <c r="Y29" s="34">
         <f>B27-SUM(C28:Y28)</f>
         <v>5.36666666666666</v>
       </c>
-      <c r="Z29" s="91">
+      <c r="Z29" s="34">
         <f>B27-SUM(C28:Z28)</f>
         <v>4.5999999999999943</v>
       </c>
-      <c r="AA29" s="91">
+      <c r="AA29" s="34">
         <f>B27-SUM(C28:AA28)</f>
         <v>3.8333333333333286</v>
       </c>
-      <c r="AB29" s="91">
+      <c r="AB29" s="34">
         <f>B27-SUM(C28:AB28)</f>
         <v>3.0666666666666629</v>
       </c>
-      <c r="AC29" s="91">
+      <c r="AC29" s="34">
         <f>B27-SUM(C28:AC28)</f>
         <v>2.2999999999999972</v>
       </c>
-      <c r="AD29" s="91">
+      <c r="AD29" s="34">
         <f>B27-SUM(C28:AD28)</f>
         <v>1.5333333333333314</v>
       </c>
-      <c r="AE29" s="91">
+      <c r="AE29" s="34">
         <f>B27-SUM(C28:AE28)</f>
         <v>0.76666666666666572</v>
       </c>
-      <c r="AF29" s="91">
+      <c r="AF29" s="34">
         <f>B27-SUM(C28:AF28)</f>
         <v>0</v>
       </c>
@@ -13826,14 +13789,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="70.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>58</v>
       </c>
@@ -13844,61 +13807,61 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+    <row r="2" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+    <row r="3" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103"/>
-      <c r="B4" s="103" t="s">
+    <row r="4" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="102"/>
+      <c r="B4" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="103"/>
-    </row>
-    <row r="5" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-    </row>
-    <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="103"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-    </row>
-    <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C4" s="102"/>
+    </row>
+    <row r="5" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="102"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+    </row>
+    <row r="6" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="102"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+    </row>
+    <row r="7" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13913,14 +13876,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="70.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>58</v>
       </c>
@@ -13931,61 +13894,61 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+    <row r="2" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+    <row r="3" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103"/>
-      <c r="B4" s="103" t="s">
+    <row r="4" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="102"/>
+      <c r="B4" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="103"/>
-    </row>
-    <row r="5" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-    </row>
-    <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="103"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-    </row>
-    <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C4" s="102"/>
+    </row>
+    <row r="5" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="102"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+    </row>
+    <row r="6" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="102"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+    </row>
+    <row r="7" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="39.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>